<commit_message>
Adding abilities and surges
</commit_message>
<xml_diff>
--- a/descent/src/descent.xlsx
+++ b/descent/src/descent.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="13095" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="13095" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Contenu" sheetId="8" r:id="rId1"/>
@@ -7506,13 +7506,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -13121,6 +13121,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="C24:C25"/>
@@ -13137,13 +13144,6 @@
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13158,9 +13158,9 @@
   </sheetPr>
   <dimension ref="A1:V94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R30" sqref="R30"/>
+      <selection pane="topRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18199,11 +18199,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT205"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E98" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A102" sqref="A102:Z105"/>
+      <selection pane="bottomRight" activeCell="Z142" sqref="Z142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18249,11 +18249,11 @@
       <c r="C1" s="95"/>
       <c r="D1" s="16"/>
       <c r="E1" s="32"/>
-      <c r="I1" s="431" t="s">
+      <c r="I1" s="432" t="s">
         <v>308</v>
       </c>
-      <c r="J1" s="431"/>
-      <c r="K1" s="431"/>
+      <c r="J1" s="432"/>
+      <c r="K1" s="432"/>
       <c r="M1" s="29" t="s">
         <v>221</v>
       </c>
@@ -18268,18 +18268,18 @@
       <c r="R1" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="S1" s="430" t="s">
+      <c r="S1" s="431" t="s">
         <v>261</v>
       </c>
-      <c r="T1" s="430"/>
-      <c r="U1" s="430" t="s">
+      <c r="T1" s="431"/>
+      <c r="U1" s="431" t="s">
         <v>262</v>
       </c>
-      <c r="V1" s="430"/>
-      <c r="W1" s="430" t="s">
+      <c r="V1" s="431"/>
+      <c r="W1" s="431" t="s">
         <v>263</v>
       </c>
-      <c r="X1" s="430"/>
+      <c r="X1" s="431"/>
       <c r="AA1" s="63"/>
       <c r="AB1" s="115"/>
       <c r="AC1" s="115"/>
@@ -28664,13 +28664,13 @@
       </c>
     </row>
     <row r="102" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="432" t="s">
+      <c r="A102" s="430" t="s">
         <v>1301</v>
       </c>
       <c r="B102" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C102" s="432" t="s">
+      <c r="C102" s="430" t="s">
         <v>1305</v>
       </c>
       <c r="D102" s="414" t="s">
@@ -28773,11 +28773,11 @@
       </c>
     </row>
     <row r="103" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="432"/>
+      <c r="A103" s="430"/>
       <c r="B103" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C103" s="432"/>
+      <c r="C103" s="430"/>
       <c r="D103" s="414"/>
       <c r="E103" s="417"/>
       <c r="F103" s="417"/>
@@ -28875,11 +28875,11 @@
       </c>
     </row>
     <row r="104" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="432"/>
+      <c r="A104" s="430"/>
       <c r="B104" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C104" s="432"/>
+      <c r="C104" s="430"/>
       <c r="D104" s="414"/>
       <c r="E104" s="417"/>
       <c r="F104" s="417" t="s">
@@ -28976,11 +28976,11 @@
       </c>
     </row>
     <row r="105" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="432"/>
+      <c r="A105" s="430"/>
       <c r="B105" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C105" s="432"/>
+      <c r="C105" s="430"/>
       <c r="D105" s="414"/>
       <c r="E105" s="417"/>
       <c r="F105" s="417"/>
@@ -29078,13 +29078,13 @@
       </c>
     </row>
     <row r="106" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="432" t="s">
+      <c r="A106" s="430" t="s">
         <v>1301</v>
       </c>
       <c r="B106" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C106" s="432" t="s">
+      <c r="C106" s="430" t="s">
         <v>1305</v>
       </c>
       <c r="D106" s="414" t="s">
@@ -29195,11 +29195,11 @@
       </c>
     </row>
     <row r="107" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="432"/>
+      <c r="A107" s="430"/>
       <c r="B107" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C107" s="432"/>
+      <c r="C107" s="430"/>
       <c r="D107" s="414"/>
       <c r="E107" s="417"/>
       <c r="F107" s="417"/>
@@ -29302,11 +29302,11 @@
       </c>
     </row>
     <row r="108" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="432"/>
+      <c r="A108" s="430"/>
       <c r="B108" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C108" s="432"/>
+      <c r="C108" s="430"/>
       <c r="D108" s="414"/>
       <c r="E108" s="417"/>
       <c r="F108" s="417" t="s">
@@ -29411,11 +29411,11 @@
       </c>
     </row>
     <row r="109" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="432"/>
+      <c r="A109" s="430"/>
       <c r="B109" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C109" s="432"/>
+      <c r="C109" s="430"/>
       <c r="D109" s="414"/>
       <c r="E109" s="417"/>
       <c r="F109" s="417"/>
@@ -29518,13 +29518,13 @@
       </c>
     </row>
     <row r="110" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="432" t="s">
+      <c r="A110" s="430" t="s">
         <v>1301</v>
       </c>
       <c r="B110" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C110" s="432" t="s">
+      <c r="C110" s="430" t="s">
         <v>1305</v>
       </c>
       <c r="D110" s="414" t="s">
@@ -29624,11 +29624,11 @@
       </c>
     </row>
     <row r="111" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="432"/>
+      <c r="A111" s="430"/>
       <c r="B111" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C111" s="432"/>
+      <c r="C111" s="430"/>
       <c r="D111" s="414"/>
       <c r="E111" s="417"/>
       <c r="F111" s="417"/>
@@ -29723,11 +29723,11 @@
       </c>
     </row>
     <row r="112" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="432"/>
+      <c r="A112" s="430"/>
       <c r="B112" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C112" s="432"/>
+      <c r="C112" s="430"/>
       <c r="D112" s="414"/>
       <c r="E112" s="417"/>
       <c r="F112" s="417" t="s">
@@ -29821,11 +29821,11 @@
       </c>
     </row>
     <row r="113" spans="1:46" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A113" s="432"/>
+      <c r="A113" s="430"/>
       <c r="B113" s="120" t="s">
         <v>316</v>
       </c>
-      <c r="C113" s="432"/>
+      <c r="C113" s="430"/>
       <c r="D113" s="414"/>
       <c r="E113" s="417"/>
       <c r="F113" s="417"/>
@@ -29920,13 +29920,13 @@
       </c>
     </row>
     <row r="114" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="432" t="s">
+      <c r="A114" s="430" t="s">
         <v>1300</v>
       </c>
       <c r="B114" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C114" s="432" t="s">
+      <c r="C114" s="430" t="s">
         <v>1305</v>
       </c>
       <c r="D114" s="414" t="s">
@@ -30032,11 +30032,11 @@
       </c>
     </row>
     <row r="115" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="432"/>
+      <c r="A115" s="430"/>
       <c r="B115" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C115" s="432"/>
+      <c r="C115" s="430"/>
       <c r="D115" s="414"/>
       <c r="E115" s="417"/>
       <c r="F115" s="417"/>
@@ -30137,11 +30137,11 @@
       </c>
     </row>
     <row r="116" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="432"/>
+      <c r="A116" s="430"/>
       <c r="B116" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C116" s="432"/>
+      <c r="C116" s="430"/>
       <c r="D116" s="414"/>
       <c r="E116" s="417"/>
       <c r="F116" s="417" t="s">
@@ -30241,11 +30241,11 @@
       </c>
     </row>
     <row r="117" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="432"/>
+      <c r="A117" s="430"/>
       <c r="B117" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C117" s="432"/>
+      <c r="C117" s="430"/>
       <c r="D117" s="414"/>
       <c r="E117" s="417"/>
       <c r="F117" s="417"/>
@@ -30346,13 +30346,13 @@
       </c>
     </row>
     <row r="118" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="432" t="s">
+      <c r="A118" s="430" t="s">
         <v>1300</v>
       </c>
       <c r="B118" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C118" s="432" t="s">
+      <c r="C118" s="430" t="s">
         <v>1307</v>
       </c>
       <c r="D118" s="414" t="s">
@@ -30455,11 +30455,11 @@
       </c>
     </row>
     <row r="119" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="432"/>
+      <c r="A119" s="430"/>
       <c r="B119" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C119" s="432"/>
+      <c r="C119" s="430"/>
       <c r="D119" s="414"/>
       <c r="E119" s="417"/>
       <c r="F119" s="417"/>
@@ -30557,11 +30557,11 @@
       </c>
     </row>
     <row r="120" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="432"/>
+      <c r="A120" s="430"/>
       <c r="B120" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C120" s="432"/>
+      <c r="C120" s="430"/>
       <c r="D120" s="414"/>
       <c r="E120" s="417"/>
       <c r="F120" s="417" t="s">
@@ -30658,11 +30658,11 @@
       </c>
     </row>
     <row r="121" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="432"/>
+      <c r="A121" s="430"/>
       <c r="B121" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="C121" s="432"/>
+      <c r="C121" s="430"/>
       <c r="D121" s="414"/>
       <c r="E121" s="417"/>
       <c r="F121" s="417"/>
@@ -30760,13 +30760,13 @@
       </c>
     </row>
     <row r="122" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="432" t="s">
+      <c r="A122" s="430" t="s">
         <v>1302</v>
       </c>
       <c r="B122" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C122" s="432" t="s">
+      <c r="C122" s="430" t="s">
         <v>1306</v>
       </c>
       <c r="D122" s="414" t="s">
@@ -30869,11 +30869,11 @@
       </c>
     </row>
     <row r="123" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="432"/>
+      <c r="A123" s="430"/>
       <c r="B123" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C123" s="432"/>
+      <c r="C123" s="430"/>
       <c r="D123" s="414"/>
       <c r="E123" s="417"/>
       <c r="F123" s="417"/>
@@ -30974,11 +30974,11 @@
       </c>
     </row>
     <row r="124" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="432"/>
+      <c r="A124" s="430"/>
       <c r="B124" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C124" s="432"/>
+      <c r="C124" s="430"/>
       <c r="D124" s="414"/>
       <c r="E124" s="417"/>
       <c r="F124" s="417" t="s">
@@ -31075,11 +31075,11 @@
       </c>
     </row>
     <row r="125" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="432"/>
+      <c r="A125" s="430"/>
       <c r="B125" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C125" s="432"/>
+      <c r="C125" s="430"/>
       <c r="D125" s="414"/>
       <c r="E125" s="417"/>
       <c r="F125" s="417"/>
@@ -31177,13 +31177,13 @@
       </c>
     </row>
     <row r="126" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="432" t="s">
+      <c r="A126" s="430" t="s">
         <v>1302</v>
       </c>
       <c r="B126" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C126" s="432" t="s">
+      <c r="C126" s="430" t="s">
         <v>1306</v>
       </c>
       <c r="D126" s="414" t="s">
@@ -31288,11 +31288,11 @@
       </c>
     </row>
     <row r="127" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="432"/>
+      <c r="A127" s="430"/>
       <c r="B127" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C127" s="432"/>
+      <c r="C127" s="430"/>
       <c r="D127" s="414"/>
       <c r="E127" s="417"/>
       <c r="F127" s="417"/>
@@ -31389,11 +31389,11 @@
       </c>
     </row>
     <row r="128" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="432"/>
+      <c r="A128" s="430"/>
       <c r="B128" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C128" s="432"/>
+      <c r="C128" s="430"/>
       <c r="D128" s="414"/>
       <c r="E128" s="417"/>
       <c r="F128" s="417" t="s">
@@ -31489,11 +31489,11 @@
       </c>
     </row>
     <row r="129" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="432"/>
+      <c r="A129" s="430"/>
       <c r="B129" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C129" s="432"/>
+      <c r="C129" s="430"/>
       <c r="D129" s="414"/>
       <c r="E129" s="417"/>
       <c r="F129" s="417"/>
@@ -31587,13 +31587,13 @@
       </c>
     </row>
     <row r="130" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="432" t="s">
+      <c r="A130" s="430" t="s">
         <v>1302</v>
       </c>
       <c r="B130" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C130" s="432" t="s">
+      <c r="C130" s="430" t="s">
         <v>1306</v>
       </c>
       <c r="D130" s="414" t="s">
@@ -31699,11 +31699,11 @@
       </c>
     </row>
     <row r="131" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="432"/>
+      <c r="A131" s="430"/>
       <c r="B131" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C131" s="432"/>
+      <c r="C131" s="430"/>
       <c r="D131" s="414"/>
       <c r="E131" s="417"/>
       <c r="F131" s="417"/>
@@ -31801,11 +31801,11 @@
       </c>
     </row>
     <row r="132" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="432"/>
+      <c r="A132" s="430"/>
       <c r="B132" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C132" s="432"/>
+      <c r="C132" s="430"/>
       <c r="D132" s="414"/>
       <c r="E132" s="417"/>
       <c r="F132" s="417" t="s">
@@ -31902,11 +31902,11 @@
       </c>
     </row>
     <row r="133" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="432"/>
+      <c r="A133" s="430"/>
       <c r="B133" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C133" s="432"/>
+      <c r="C133" s="430"/>
       <c r="D133" s="414"/>
       <c r="E133" s="417"/>
       <c r="F133" s="417"/>
@@ -32001,13 +32001,13 @@
       </c>
     </row>
     <row r="134" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="432" t="s">
+      <c r="A134" s="430" t="s">
         <v>1302</v>
       </c>
       <c r="B134" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C134" s="432" t="s">
+      <c r="C134" s="430" t="s">
         <v>1308</v>
       </c>
       <c r="D134" s="414" t="s">
@@ -32110,11 +32110,11 @@
       </c>
     </row>
     <row r="135" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="432"/>
+      <c r="A135" s="430"/>
       <c r="B135" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C135" s="432"/>
+      <c r="C135" s="430"/>
       <c r="D135" s="414"/>
       <c r="E135" s="417"/>
       <c r="F135" s="417"/>
@@ -32212,11 +32212,11 @@
       </c>
     </row>
     <row r="136" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="432"/>
+      <c r="A136" s="430"/>
       <c r="B136" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C136" s="432"/>
+      <c r="C136" s="430"/>
       <c r="D136" s="414"/>
       <c r="E136" s="417"/>
       <c r="F136" s="417" t="s">
@@ -32313,11 +32313,11 @@
       </c>
     </row>
     <row r="137" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="432"/>
+      <c r="A137" s="430"/>
       <c r="B137" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="C137" s="432"/>
+      <c r="C137" s="430"/>
       <c r="D137" s="414"/>
       <c r="E137" s="417"/>
       <c r="F137" s="417"/>
@@ -32412,13 +32412,13 @@
       </c>
     </row>
     <row r="138" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="432" t="s">
+      <c r="A138" s="430" t="s">
         <v>1304</v>
       </c>
       <c r="B138" s="120" t="s">
         <v>1465</v>
       </c>
-      <c r="C138" s="432" t="s">
+      <c r="C138" s="430" t="s">
         <v>1305</v>
       </c>
       <c r="D138" s="414" t="s">
@@ -32527,11 +32527,11 @@
       </c>
     </row>
     <row r="139" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="432"/>
+      <c r="A139" s="430"/>
       <c r="B139" s="120" t="s">
         <v>1465</v>
       </c>
-      <c r="C139" s="432"/>
+      <c r="C139" s="430"/>
       <c r="D139" s="414"/>
       <c r="E139" s="417"/>
       <c r="F139" s="417"/>
@@ -32632,11 +32632,11 @@
       </c>
     </row>
     <row r="140" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="432"/>
+      <c r="A140" s="430"/>
       <c r="B140" s="120" t="s">
         <v>1465</v>
       </c>
-      <c r="C140" s="432"/>
+      <c r="C140" s="430"/>
       <c r="D140" s="414"/>
       <c r="E140" s="417"/>
       <c r="F140" s="417" t="s">
@@ -32739,11 +32739,11 @@
       </c>
     </row>
     <row r="141" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="432"/>
+      <c r="A141" s="430"/>
       <c r="B141" s="120" t="s">
         <v>1465</v>
       </c>
-      <c r="C141" s="432"/>
+      <c r="C141" s="430"/>
       <c r="D141" s="414"/>
       <c r="E141" s="417"/>
       <c r="F141" s="417"/>
@@ -32844,13 +32844,13 @@
       </c>
     </row>
     <row r="142" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="432" t="s">
+      <c r="A142" s="430" t="s">
         <v>1299</v>
       </c>
       <c r="B142" s="120" t="s">
         <v>313</v>
       </c>
-      <c r="C142" s="432" t="s">
+      <c r="C142" s="430" t="s">
         <v>1305</v>
       </c>
       <c r="D142" s="414" t="s">
@@ -32954,11 +32954,11 @@
       </c>
     </row>
     <row r="143" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="432"/>
+      <c r="A143" s="430"/>
       <c r="B143" s="120" t="s">
         <v>313</v>
       </c>
-      <c r="C143" s="432"/>
+      <c r="C143" s="430"/>
       <c r="D143" s="414"/>
       <c r="E143" s="417"/>
       <c r="F143" s="417"/>
@@ -33054,11 +33054,11 @@
       </c>
     </row>
     <row r="144" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="432"/>
+      <c r="A144" s="430"/>
       <c r="B144" s="120" t="s">
         <v>313</v>
       </c>
-      <c r="C144" s="432"/>
+      <c r="C144" s="430"/>
       <c r="D144" s="414"/>
       <c r="E144" s="417"/>
       <c r="F144" s="417" t="s">
@@ -33150,11 +33150,11 @@
       </c>
     </row>
     <row r="145" spans="1:46" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="432"/>
+      <c r="A145" s="430"/>
       <c r="B145" s="120" t="s">
         <v>313</v>
       </c>
-      <c r="C145" s="432"/>
+      <c r="C145" s="430"/>
       <c r="D145" s="414"/>
       <c r="E145" s="417"/>
       <c r="F145" s="417"/>
@@ -39393,90 +39393,208 @@
     <filterColumn colId="22" showButton="0"/>
   </autoFilter>
   <mergeCells count="310">
-    <mergeCell ref="A198:A201"/>
-    <mergeCell ref="C198:C201"/>
-    <mergeCell ref="D198:D201"/>
-    <mergeCell ref="E198:E201"/>
-    <mergeCell ref="F198:F199"/>
-    <mergeCell ref="F200:F201"/>
-    <mergeCell ref="A202:A205"/>
-    <mergeCell ref="C202:C205"/>
-    <mergeCell ref="D202:D205"/>
-    <mergeCell ref="E202:E205"/>
-    <mergeCell ref="F202:F203"/>
-    <mergeCell ref="F204:F205"/>
-    <mergeCell ref="A190:A193"/>
-    <mergeCell ref="C190:C193"/>
-    <mergeCell ref="D190:D193"/>
-    <mergeCell ref="E190:E193"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="F192:F193"/>
-    <mergeCell ref="A194:A197"/>
-    <mergeCell ref="C194:C197"/>
-    <mergeCell ref="D194:D197"/>
-    <mergeCell ref="E194:E197"/>
-    <mergeCell ref="F194:F195"/>
-    <mergeCell ref="F196:F197"/>
-    <mergeCell ref="A182:A185"/>
-    <mergeCell ref="C182:C185"/>
-    <mergeCell ref="D182:D185"/>
-    <mergeCell ref="E182:E185"/>
-    <mergeCell ref="F182:F183"/>
-    <mergeCell ref="F184:F185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="C186:C189"/>
-    <mergeCell ref="D186:D189"/>
-    <mergeCell ref="E186:E189"/>
-    <mergeCell ref="F186:F187"/>
-    <mergeCell ref="F188:F189"/>
-    <mergeCell ref="A166:A169"/>
-    <mergeCell ref="C166:C169"/>
-    <mergeCell ref="D166:D169"/>
-    <mergeCell ref="E166:E169"/>
-    <mergeCell ref="F166:F167"/>
-    <mergeCell ref="F168:F169"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="D158:D161"/>
-    <mergeCell ref="E158:E161"/>
-    <mergeCell ref="F158:F159"/>
-    <mergeCell ref="F160:F161"/>
-    <mergeCell ref="A162:A165"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="D162:D165"/>
-    <mergeCell ref="E162:E165"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="F164:F165"/>
-    <mergeCell ref="A98:A101"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D101"/>
-    <mergeCell ref="E98:E101"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D93"/>
-    <mergeCell ref="E90:E93"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="D94:D97"/>
-    <mergeCell ref="E94:E97"/>
-    <mergeCell ref="F94:F95"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D85"/>
-    <mergeCell ref="E82:E85"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D86:D89"/>
-    <mergeCell ref="E86:E89"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="C178:C181"/>
+    <mergeCell ref="D178:D181"/>
+    <mergeCell ref="E178:E181"/>
+    <mergeCell ref="F178:F179"/>
+    <mergeCell ref="F180:F181"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="D170:D173"/>
+    <mergeCell ref="E170:E173"/>
+    <mergeCell ref="F170:F171"/>
+    <mergeCell ref="F172:F173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="C174:C177"/>
+    <mergeCell ref="D174:D177"/>
+    <mergeCell ref="E174:E177"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="F176:F177"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="D78:D81"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="F80:F81"/>
+    <mergeCell ref="A154:A157"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="D154:D157"/>
+    <mergeCell ref="E154:E157"/>
+    <mergeCell ref="F154:F155"/>
+    <mergeCell ref="F156:F157"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="A146:A149"/>
+    <mergeCell ref="C146:C149"/>
+    <mergeCell ref="D146:D149"/>
+    <mergeCell ref="E146:E149"/>
+    <mergeCell ref="F146:F147"/>
+    <mergeCell ref="F148:F149"/>
+    <mergeCell ref="A150:A153"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="D150:D153"/>
+    <mergeCell ref="E150:E153"/>
+    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="E134:E137"/>
+    <mergeCell ref="D138:D141"/>
+    <mergeCell ref="D142:D145"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="F140:F141"/>
+    <mergeCell ref="F142:F143"/>
+    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="E110:E113"/>
+    <mergeCell ref="E114:E117"/>
+    <mergeCell ref="E118:E121"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="E126:E129"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="D134:D137"/>
+    <mergeCell ref="E138:E141"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="F122:F123"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="E142:E145"/>
+    <mergeCell ref="D126:D129"/>
+    <mergeCell ref="E130:E133"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="D102:D105"/>
+    <mergeCell ref="D106:D109"/>
+    <mergeCell ref="F102:F103"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="F112:F113"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="D130:D133"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="E102:E105"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="D110:D113"/>
+    <mergeCell ref="D114:D117"/>
+    <mergeCell ref="D118:D121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="A142:A145"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="A122:A125"/>
+    <mergeCell ref="A126:A129"/>
     <mergeCell ref="C130:C133"/>
     <mergeCell ref="C134:C137"/>
     <mergeCell ref="C138:C141"/>
@@ -39501,208 +39619,90 @@
     <mergeCell ref="C102:C105"/>
     <mergeCell ref="C106:C109"/>
     <mergeCell ref="C110:C113"/>
-    <mergeCell ref="A142:A145"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A102:A105"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="A110:A113"/>
-    <mergeCell ref="A114:A117"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A118:A121"/>
-    <mergeCell ref="A122:A125"/>
-    <mergeCell ref="A126:A129"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="F110:F111"/>
-    <mergeCell ref="F112:F113"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="D130:D133"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="E102:E105"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="D110:D113"/>
-    <mergeCell ref="D114:D117"/>
-    <mergeCell ref="D118:D121"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="D102:D105"/>
-    <mergeCell ref="D106:D109"/>
-    <mergeCell ref="F102:F103"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="E134:E137"/>
-    <mergeCell ref="D138:D141"/>
-    <mergeCell ref="D142:D145"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="F140:F141"/>
-    <mergeCell ref="F142:F143"/>
-    <mergeCell ref="F144:F145"/>
-    <mergeCell ref="E110:E113"/>
-    <mergeCell ref="E114:E117"/>
-    <mergeCell ref="E118:E121"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="E126:E129"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="D134:D137"/>
-    <mergeCell ref="E138:E141"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="F122:F123"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="E142:E145"/>
-    <mergeCell ref="D126:D129"/>
-    <mergeCell ref="E130:E133"/>
-    <mergeCell ref="A146:A149"/>
-    <mergeCell ref="C146:C149"/>
-    <mergeCell ref="D146:D149"/>
-    <mergeCell ref="E146:E149"/>
-    <mergeCell ref="F146:F147"/>
-    <mergeCell ref="F148:F149"/>
-    <mergeCell ref="A150:A153"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="D150:D153"/>
-    <mergeCell ref="E150:E153"/>
-    <mergeCell ref="F150:F151"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A154:A157"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D157"/>
-    <mergeCell ref="E154:E157"/>
-    <mergeCell ref="F154:F155"/>
-    <mergeCell ref="F156:F157"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="E74:E77"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="D78:D81"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="F80:F81"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="C178:C181"/>
-    <mergeCell ref="D178:D181"/>
-    <mergeCell ref="E178:E181"/>
-    <mergeCell ref="F178:F179"/>
-    <mergeCell ref="F180:F181"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="D170:D173"/>
-    <mergeCell ref="E170:E173"/>
-    <mergeCell ref="F170:F171"/>
-    <mergeCell ref="F172:F173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="C174:C177"/>
-    <mergeCell ref="D174:D177"/>
-    <mergeCell ref="E174:E177"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="F176:F177"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D85"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D86:D89"/>
+    <mergeCell ref="E86:E89"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D101"/>
+    <mergeCell ref="E98:E101"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D93"/>
+    <mergeCell ref="E90:E93"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="D94:D97"/>
+    <mergeCell ref="E94:E97"/>
+    <mergeCell ref="F94:F95"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="A166:A169"/>
+    <mergeCell ref="C166:C169"/>
+    <mergeCell ref="D166:D169"/>
+    <mergeCell ref="E166:E169"/>
+    <mergeCell ref="F166:F167"/>
+    <mergeCell ref="F168:F169"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="D158:D161"/>
+    <mergeCell ref="E158:E161"/>
+    <mergeCell ref="F158:F159"/>
+    <mergeCell ref="F160:F161"/>
+    <mergeCell ref="A162:A165"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="D162:D165"/>
+    <mergeCell ref="E162:E165"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="F164:F165"/>
+    <mergeCell ref="A182:A185"/>
+    <mergeCell ref="C182:C185"/>
+    <mergeCell ref="D182:D185"/>
+    <mergeCell ref="E182:E185"/>
+    <mergeCell ref="F182:F183"/>
+    <mergeCell ref="F184:F185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="C186:C189"/>
+    <mergeCell ref="D186:D189"/>
+    <mergeCell ref="E186:E189"/>
+    <mergeCell ref="F186:F187"/>
+    <mergeCell ref="F188:F189"/>
+    <mergeCell ref="A190:A193"/>
+    <mergeCell ref="C190:C193"/>
+    <mergeCell ref="D190:D193"/>
+    <mergeCell ref="E190:E193"/>
+    <mergeCell ref="F190:F191"/>
+    <mergeCell ref="F192:F193"/>
+    <mergeCell ref="A194:A197"/>
+    <mergeCell ref="C194:C197"/>
+    <mergeCell ref="D194:D197"/>
+    <mergeCell ref="E194:E197"/>
+    <mergeCell ref="F194:F195"/>
+    <mergeCell ref="F196:F197"/>
+    <mergeCell ref="A198:A201"/>
+    <mergeCell ref="C198:C201"/>
+    <mergeCell ref="D198:D201"/>
+    <mergeCell ref="E198:E201"/>
+    <mergeCell ref="F198:F199"/>
+    <mergeCell ref="F200:F201"/>
+    <mergeCell ref="A202:A205"/>
+    <mergeCell ref="C202:C205"/>
+    <mergeCell ref="D202:D205"/>
+    <mergeCell ref="E202:E205"/>
+    <mergeCell ref="F202:F203"/>
+    <mergeCell ref="F204:F205"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39716,8 +39716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -44343,9 +44343,9 @@
   <dimension ref="A1:R144"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3600" topLeftCell="A102" activePane="bottomLeft"/>
+      <pane ySplit="3600" topLeftCell="A13" activePane="bottomLeft"/>
       <selection activeCell="Q52" sqref="Q52"/>
-      <selection pane="bottomLeft" activeCell="R25" sqref="R25:R114"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -50355,6 +50355,11 @@
   </sortState>
   <dataConsolidate/>
   <mergeCells count="21">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E1:F1"/>
@@ -50371,11 +50376,6 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:D25 F25:H25 C47:H47">
     <cfRule type="expression" dxfId="151" priority="149">

</xml_diff>